<commit_message>
Change the error message
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/data.xlsx
+++ b/src/test/resources/TestData/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e33941310077015d/Documents/selenium_2024/CucumberFramework/src/test/resources/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="11_F25DC773A252ABDACC10486E399E501A5BDE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59E8C6F8-66B0-425F-B12C-0E775ACC00EC}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="11_F25DC773A252ABDACC10486E399E501A5BDE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{217F7EAD-26E6-43CA-A50B-2CE7DF823A3E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,12 +48,6 @@
     <t>sbi</t>
   </si>
   <si>
-    <t>Userid</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
     <t>Fstname</t>
   </si>
   <si>
@@ -73,6 +67,12 @@
   </si>
   <si>
     <t>TC03_lead_creation</t>
+  </si>
+  <si>
+    <t>userid</t>
+  </si>
+  <si>
+    <t>password</t>
   </si>
 </sst>
 </file>
@@ -428,7 +428,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -443,27 +443,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -478,7 +478,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -493,7 +493,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>1</v>

</xml_diff>